<commit_message>
add self for motor, unified footprints capa resistor
git-svn-id: file:///Users/administrator/mobots/svn/electronics/thymio2/trunk@697 56f7f59e-b348-0410-8d88-ca71a75c094d
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="14625"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials by layers-thy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="269">
   <si>
     <t>Quantity</t>
   </si>
@@ -67,21 +67,24 @@
     <t>Capacitor</t>
   </si>
   <si>
+    <t>CAPC1608X08L</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
     <t>RESC1608X06L</t>
   </si>
   <si>
-    <t>6.2</t>
-  </si>
-  <si>
-    <t>RES</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>815-ABLS-8-B2</t>
   </si>
   <si>
@@ -223,31 +226,31 @@
     <t>Led_TH_3mm_20mm</t>
   </si>
   <si>
+    <t>MC74HC595ADTR2</t>
+  </si>
+  <si>
+    <t>U13, U15, U17</t>
+  </si>
+  <si>
+    <t>8-Bit Serial-Input/Serial or Prallel-Output Shift Register with Latched 3-State Outputs</t>
+  </si>
+  <si>
+    <t>948F-01_N</t>
+  </si>
+  <si>
+    <t>1.5K</t>
+  </si>
+  <si>
+    <t>R17, R18, R19, R20</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>4.7uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>C51, C52, C72</t>
-  </si>
-  <si>
-    <t>MC74HC595ADTR2</t>
-  </si>
-  <si>
-    <t>U13, U15, U17</t>
-  </si>
-  <si>
-    <t>8-Bit Serial-Input/Serial or Prallel-Output Shift Register with Latched 3-State Outputs</t>
-  </si>
-  <si>
-    <t>948F-01_N</t>
-  </si>
-  <si>
-    <t>1.5K</t>
-  </si>
-  <si>
-    <t>R17, R18, R19, R20</t>
+    <t>10uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1, 4.7uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1</t>
+  </si>
+  <si>
+    <t>C51, C52, C72, C73</t>
   </si>
   <si>
     <t>1K</t>
@@ -262,6 +265,15 @@
     <t>R7, R8, R9, R10</t>
   </si>
   <si>
+    <t>820</t>
+  </si>
+  <si>
+    <t>22K[[/\]]0603[[/\]]1</t>
+  </si>
+  <si>
+    <t>R151, R152, R153, R154</t>
+  </si>
+  <si>
     <t>DMG1012T</t>
   </si>
   <si>
@@ -283,6 +295,21 @@
     <t>Transistor MOSFET 1 x P Pining : 1=G, 2=S, 3=D</t>
   </si>
   <si>
+    <t>MLP2520S3R3S</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>L1, L2, L3, L4</t>
+  </si>
+  <si>
+    <t>Inductors for Power Circuits  Multilayer/STD  Magnetic Shielded</t>
+  </si>
+  <si>
+    <t>INDC2520X12L</t>
+  </si>
+  <si>
     <t>100K</t>
   </si>
   <si>
@@ -310,36 +337,39 @@
     <t>C15, C16, C17, C18, C19, C20, C21</t>
   </si>
   <si>
-    <t>CAPC1608N</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
-    <t>10K[[/\]]0603[[/\]]2, RES</t>
+    <t>RES, RES, RES, RES, RES, RES, RES, 10K[[/\]]0603[[/\]]2</t>
   </si>
   <si>
     <t>R27, R28, R29, R30, R31, R50, R51, R136</t>
   </si>
   <si>
-    <t>120, Resistor</t>
+    <t>120, 120, 120, 120, 120, 120, 120, Resistor</t>
   </si>
   <si>
     <t>2.2K</t>
   </si>
   <si>
-    <t>2.2K[[/\]]0603[[/\]]1, RES</t>
+    <t>RES, RES, RES, RES, RES, 2.2K[[/\]]0603[[/\]]1, RES, RES</t>
   </si>
   <si>
     <t>R12, R13, R14, R15, R16, R33, R44, R45</t>
   </si>
   <si>
+    <t>120, 120, 120, 120, 120, Resistor, 120, 120</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
     <t>R3, R5, R68, R69, R70, R71, R72, R73</t>
   </si>
   <si>
+    <t>120, Resistor, 120, 120, 120, 120, 120, 120</t>
+  </si>
+  <si>
     <t>39</t>
   </si>
   <si>
@@ -394,9 +424,6 @@
     <t>47K</t>
   </si>
   <si>
-    <t>22K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R132</t>
   </si>
   <si>
@@ -424,9 +451,6 @@
     <t>R125</t>
   </si>
   <si>
-    <t>820</t>
-  </si>
-  <si>
     <t>R131</t>
   </si>
   <si>
@@ -613,7 +637,7 @@
     <t>Omnidirectional Back Electret Condenser Microphone</t>
   </si>
   <si>
-    <t>MICRO_PANASONIC_WM-64PN</t>
+    <t>MICRO_TD4015BPN</t>
   </si>
   <si>
     <t>R67, R92, R93, R94, R103, R104, R142, R144, R145, R146</t>
@@ -634,7 +658,7 @@
     <t>C53, C54</t>
   </si>
   <si>
-    <t>1uF[[/\]]0603[[/\]]1, 4.7uF[[/\]]0603[[/\]]1</t>
+    <t>4.7uF[[/\]]0603[[/\]]1, 1uF[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>C56, C61</t>
@@ -673,9 +697,6 @@
     <t>Motor, General Kind</t>
   </si>
   <si>
-    <t>RB5-10.5</t>
-  </si>
-  <si>
     <t>C1, C3, C6, C10, C11, C12, C13, C23, C24, C27, C29, C33, C35, C36, C37, C38, C39, C62, C65, C66, C67</t>
   </si>
   <si>
@@ -703,7 +724,7 @@
     <t>47nF</t>
   </si>
   <si>
-    <t>10nF[[/\]]0603[[/\]]1, 470nF[[/\]]0603[[/\]]1</t>
+    <t>470nF[[/\]]0603[[/\]]1, 10nF[[/\]]0603[[/\]]1, 470nF[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>C58, C59, C60</t>
@@ -724,7 +745,7 @@
     <t>DIOC1608X08N</t>
   </si>
   <si>
-    <t>10K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1</t>
+    <t>100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>R138, R139, R141, R143</t>
@@ -742,13 +763,16 @@
     <t>SMD Red 0603 2V@20ma 56 mcd</t>
   </si>
   <si>
-    <t>1K[[/\]]0603[[/\]]1, RES</t>
+    <t>RES, RES, RES, 1K[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>R25, R48, R49, R108</t>
   </si>
   <si>
-    <t>22K[[/\]]0603[[/\]]1, RES</t>
+    <t>120, 120, 120, Resistor</t>
+  </si>
+  <si>
+    <t>RES, RES, RES, 22K[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>R11, R42, R43, R130</t>
@@ -772,16 +796,19 @@
     <t>ITR9909_EDGE</t>
   </si>
   <si>
-    <t>8.2K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]2</t>
+    <t>10K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1, 8.2K[[/\]]0603[[/\]]2, 8.2K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>R101, R102, R109, R110, R117, R118, R128, R129</t>
   </si>
   <si>
-    <t>68K[[/\]]0603[[/\]]1, RES</t>
+    <t>RES, RES, RES, 68K[[/\]]0603[[/\]]1, RES, RES, RES, 68K[[/\]]0603[[/\]]1</t>
   </si>
   <si>
     <t>R98, R99, R100, R135, R147, R148, R149, R150</t>
+  </si>
+  <si>
+    <t>120, 120, 120, Resistor, 120, 120, 120, Resistor</t>
   </si>
   <si>
     <t>R56, R58, R60, R62, R78, R79, R80, R81</t>
@@ -1164,19 +1191,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="120.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="102.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,7 +1292,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1276,19 +1303,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1299,19 +1326,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>12</v>
@@ -1322,19 +1349,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1345,19 +1372,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -1368,13 +1395,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
@@ -1391,19 +1418,19 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -1414,16 +1441,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -1437,19 +1464,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>12</v>
@@ -1460,13 +1487,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>16</v>
@@ -1483,19 +1510,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>12</v>
@@ -1506,19 +1533,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
@@ -1529,19 +1556,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>12</v>
@@ -1552,7 +1579,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>70</v>
@@ -1561,10 +1588,10 @@
         <v>71</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
@@ -1572,22 +1599,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>12</v>
@@ -1601,13 +1628,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -1621,19 +1648,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>12</v>
@@ -1644,19 +1671,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
@@ -1667,19 +1694,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
@@ -1702,7 +1729,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
@@ -1710,10 +1737,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>90</v>
@@ -1722,10 +1749,10 @@
         <v>91</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>12</v>
@@ -1733,22 +1760,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
@@ -1756,22 +1783,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>12</v>
@@ -1779,22 +1806,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
@@ -1802,19 +1829,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>17</v>
@@ -1828,19 +1855,19 @@
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>12</v>
@@ -1851,19 +1878,19 @@
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>12</v>
@@ -1871,22 +1898,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>12</v>
@@ -1894,48 +1921,48 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1943,13 +1970,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>16</v>
@@ -1958,7 +1985,7 @@
         <v>17</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,22 +1993,22 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1989,22 +2016,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2012,22 +2039,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2035,22 +2062,22 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2058,22 +2085,22 @@
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2081,22 +2108,22 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2104,22 +2131,22 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,22 +2154,22 @@
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>146</v>
+        <v>22</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>147</v>
@@ -2165,7 +2192,7 @@
         <v>150</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2188,7 +2215,7 @@
         <v>154</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2199,19 +2226,19 @@
         <v>155</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="G45" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,22 +2246,22 @@
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="G46" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2242,22 +2269,22 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2265,22 +2292,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2288,22 +2315,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>169</v>
+        <v>32</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>172</v>
+        <v>34</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>173</v>
+        <v>35</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2311,22 +2338,22 @@
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="G50" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2334,22 +2361,22 @@
         <v>1</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="G51" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2357,22 +2384,22 @@
         <v>1</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2380,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>187</v>
@@ -2395,7 +2422,7 @@
         <v>190</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2418,7 +2445,7 @@
         <v>194</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,88 +2456,88 @@
         <v>195</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="G55" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>36</v>
+        <v>199</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>200</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>38</v>
+        <v>201</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>17</v>
+        <v>202</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>38</v>
+        <v>206</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2518,22 +2545,22 @@
         <v>2</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2541,22 +2568,22 @@
         <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>209</v>
+        <v>41</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2564,22 +2591,22 @@
         <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>213</v>
+        <v>16</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2587,22 +2614,22 @@
         <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>55</v>
+        <v>216</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>56</v>
+        <v>217</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2610,22 +2637,22 @@
         <v>2</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>72</v>
+        <v>219</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>72</v>
+        <v>219</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2633,114 +2660,114 @@
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>216</v>
+        <v>56</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>216</v>
+        <v>57</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>218</v>
+        <v>59</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>219</v>
+        <v>60</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>44</v>
+        <v>226</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>223</v>
+        <v>43</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>226</v>
+        <v>46</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2748,22 +2775,22 @@
         <v>3</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2771,22 +2798,22 @@
         <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>229</v>
+        <v>66</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2794,22 +2821,22 @@
         <v>3</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2817,68 +2844,68 @@
         <v>3</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>65</v>
+        <v>236</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>234</v>
+        <v>16</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>235</v>
+        <v>17</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>236</v>
+        <v>28</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>16</v>
+        <v>241</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>17</v>
+        <v>242</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2886,22 +2913,22 @@
         <v>4</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>239</v>
+        <v>98</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>65</v>
+        <v>243</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>241</v>
+        <v>39</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>235</v>
+        <v>22</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2909,22 +2936,22 @@
         <v>4</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>242</v>
+        <v>77</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2932,114 +2959,114 @@
         <v>4</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>80</v>
+        <v>246</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>244</v>
+        <v>66</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>102</v>
+        <v>248</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>17</v>
+        <v>242</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>93</v>
+        <v>249</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>38</v>
+        <v>251</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3047,68 +3074,68 @@
         <v>7</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>60</v>
+        <v>217</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>251</v>
+        <v>22</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>252</v>
+        <v>54</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>17</v>
+        <v>259</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3116,22 +3143,22 @@
         <v>8</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>93</v>
+        <v>260</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3139,22 +3166,68 @@
         <v>8</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>257</v>
+        <v>115</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>65</v>
+        <v>262</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>235</v>
+        <v>22</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>8</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>8</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
output version 1.61 send to ACI with new connector for motors and battery
git-svn-id: file:///Users/administrator/mobots/svn/electronics/thymio2/trunk@698 56f7f59e-b348-0410-8d88-ca71a75c094d
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="14370"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="14625"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials by layers-thy" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="271">
   <si>
     <t>Quantity</t>
   </si>
@@ -112,6 +112,21 @@
     <t>SOT95P285X100-5N</t>
   </si>
   <si>
+    <t>Battery connector 89400-0220</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>Multicell Battery</t>
+  </si>
+  <si>
+    <t>BAT-2</t>
+  </si>
+  <si>
     <t>MCP6L04T-E/ST</t>
   </si>
   <si>
@@ -211,6 +226,18 @@
     <t>ITR9909_LONG</t>
   </si>
   <si>
+    <t>Motor connector 89400-0220</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>B1, B2</t>
+  </si>
+  <si>
+    <t>Motor, General Kind</t>
+  </si>
+  <si>
     <t>WP7104SRC/D</t>
   </si>
   <si>
@@ -469,18 +496,6 @@
     <t>Astron 3190005-x21-r</t>
   </si>
   <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>Multicell Battery</t>
-  </si>
-  <si>
-    <t>BAT-2</t>
-  </si>
-  <si>
     <t>Con1x6</t>
   </si>
   <si>
@@ -686,15 +701,6 @@
   </si>
   <si>
     <t>U14, U16</t>
-  </si>
-  <si>
-    <t>Motor</t>
-  </si>
-  <si>
-    <t>B1, B2</t>
-  </si>
-  <si>
-    <t>Motor, General Kind</t>
   </si>
   <si>
     <t>C1, C3, C6, C10, C11, C12, C13, C23, C24, C27, C29, C33, C35, C36, C37, C38, C39, C62, C65, C66, C67</t>
@@ -1352,16 +1358,16 @@
         <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1369,10 +1375,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>37</v>
@@ -1384,7 +1390,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -1392,22 +1398,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -1415,22 +1421,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -1438,10 +1444,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>48</v>
@@ -1453,7 +1459,7 @@
         <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
@@ -1464,19 +1470,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>12</v>
@@ -1487,19 +1493,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>12</v>
@@ -1510,19 +1516,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>12</v>
@@ -1536,16 +1542,16 @@
         <v>61</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
@@ -1556,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
@@ -1576,22 +1582,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
@@ -1599,22 +1605,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>12</v>
@@ -1622,22 +1628,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>12</v>
@@ -1648,13 +1654,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>21</v>
@@ -1671,19 +1677,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
@@ -1694,16 +1700,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>22</v>
@@ -1717,19 +1723,19 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
@@ -1740,19 +1746,19 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>12</v>
@@ -1763,19 +1769,19 @@
         <v>4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
@@ -1783,10 +1789,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>99</v>
@@ -1795,10 +1801,10 @@
         <v>100</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>12</v>
@@ -1806,22 +1812,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
@@ -1829,22 +1835,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>12</v>
@@ -1852,19 +1858,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>22</v>
@@ -1875,22 +1881,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>12</v>
@@ -1901,16 +1907,16 @@
         <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>22</v>
@@ -1924,16 +1930,16 @@
         <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>22</v>
@@ -1944,22 +1950,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>12</v>
@@ -1967,48 +1973,48 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2016,13 +2022,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -2031,7 +2037,7 @@
         <v>17</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2039,22 +2045,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2062,22 +2068,22 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2085,22 +2091,22 @@
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2108,22 +2114,22 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2131,22 +2137,22 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2154,22 +2160,22 @@
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,22 +2183,22 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>149</v>
+        <v>44</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2200,22 +2206,22 @@
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2226,19 +2232,19 @@
         <v>155</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2246,22 +2252,22 @@
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2269,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>164</v>
@@ -2284,7 +2290,7 @@
         <v>167</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,19 +2301,19 @@
         <v>168</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2315,22 +2321,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2338,22 +2344,22 @@
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2361,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>178</v>
@@ -2376,7 +2382,7 @@
         <v>181</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2387,19 +2393,19 @@
         <v>182</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>187</v>
@@ -2422,7 +2428,7 @@
         <v>190</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2433,19 +2439,19 @@
         <v>191</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2453,22 +2459,22 @@
         <v>1</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2476,22 +2482,22 @@
         <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2499,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>204</v>
@@ -2514,53 +2520,53 @@
         <v>207</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>37</v>
+        <v>209</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>209</v>
+        <v>41</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>210</v>
+        <v>42</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2568,22 +2574,22 @@
         <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>41</v>
+        <v>215</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2591,13 +2597,13 @@
         <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>13</v>
+        <v>217</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>214</v>
+        <v>46</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>16</v>
@@ -2606,7 +2612,7 @@
         <v>17</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2614,22 +2620,22 @@
         <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>216</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2637,22 +2643,22 @@
         <v>2</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>221</v>
+        <v>44</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2660,22 +2666,22 @@
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>56</v>
+        <v>224</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>57</v>
+        <v>224</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>59</v>
+        <v>226</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2683,22 +2689,22 @@
         <v>2</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2706,22 +2712,22 @@
         <v>2</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>224</v>
+        <v>79</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>224</v>
+        <v>79</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>226</v>
+        <v>81</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2729,13 +2735,13 @@
         <v>21</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>16</v>
@@ -2744,7 +2750,7 @@
         <v>17</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2752,22 +2758,22 @@
         <v>28</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2775,13 +2781,13 @@
         <v>3</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>21</v>
@@ -2790,7 +2796,7 @@
         <v>22</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,22 +2804,22 @@
         <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2821,22 +2827,22 @@
         <v>3</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2844,13 +2850,13 @@
         <v>3</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>16</v>
@@ -2859,7 +2865,7 @@
         <v>17</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,7 +2879,7 @@
         <v>28</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>30</v>
@@ -2882,7 +2888,7 @@
         <v>31</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,22 +2896,22 @@
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2913,22 +2919,22 @@
         <v>4</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2936,13 +2942,13 @@
         <v>4</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>16</v>
@@ -2951,7 +2957,7 @@
         <v>17</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2959,22 +2965,22 @@
         <v>4</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2982,22 +2988,22 @@
         <v>4</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3005,22 +3011,22 @@
         <v>4</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D79" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3028,22 +3034,22 @@
         <v>6</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3057,7 +3063,7 @@
         <v>19</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>21</v>
@@ -3066,7 +3072,7 @@
         <v>22</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3074,22 +3080,22 @@
         <v>7</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3097,13 +3103,13 @@
         <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>16</v>
@@ -3112,7 +3118,7 @@
         <v>17</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3120,22 +3126,22 @@
         <v>7</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3143,22 +3149,22 @@
         <v>8</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3166,22 +3172,22 @@
         <v>8</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3189,22 +3195,22 @@
         <v>8</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3212,22 +3218,22 @@
         <v>8</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapt resistance for production
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="221">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -283,18 +283,18 @@
     <t xml:space="preserve">INDC2520X12L</t>
   </si>
   <si>
+    <t xml:space="preserve">4.7K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2, R111, R112, R113, R114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R74, R75, R76, R77, R90, R91</t>
+  </si>
+  <si>
     <t xml:space="preserve">R68, R69, R70, R71, R72, R73</t>
   </si>
   <si>
-    <t xml:space="preserve">4.7K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2, R111, R112, R113, R114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R74, R75, R76, R77, R90, R91</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.7nF</t>
   </si>
   <si>
@@ -556,6 +556,9 @@
     <t xml:space="preserve">R135, R150</t>
   </si>
   <si>
+    <t xml:space="preserve">R107, R137</t>
+  </si>
+  <si>
     <t xml:space="preserve">1nF</t>
   </si>
   <si>
@@ -652,6 +655,9 @@
     <t xml:space="preserve">R36, R37, R39, R40, R54, R55</t>
   </si>
   <si>
+    <t xml:space="preserve">R98, R99, R100, R147, R148, R149</t>
+  </si>
+  <si>
     <t xml:space="preserve">C32, C44, C45, C47, C48, C49, C50</t>
   </si>
   <si>
@@ -662,12 +668,6 @@
   </si>
   <si>
     <t xml:space="preserve">R101, R102, R109, R110, R117, R118, R128, R129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R98, R99, R100, R107, R137, R147, R148, R149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180, 180, 180, Resistor, Resistor, 180, 180, 180</t>
   </si>
   <si>
     <t xml:space="preserve">R56, R58, R60, R62, R78, R79, R80, R81</t>
@@ -778,7 +778,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1353,14 +1353,14 @@
       <c r="A30" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>180</v>
+      <c r="B30" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>180</v>
+        <v>88</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>15</v>
@@ -1373,8 +1373,8 @@
       <c r="A31" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>88</v>
+      <c r="B31" s="0" t="n">
+        <v>56</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>89</v>
@@ -1394,13 +1394,13 @@
         <v>6</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>34</v>
+      <c r="D32" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>15</v>
@@ -2033,17 +2033,17 @@
       <c r="A64" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="C64" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>179</v>
-      </c>
       <c r="D64" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>106</v>
@@ -2054,7 +2054,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>180</v>
@@ -2074,16 +2074,16 @@
         <v>2</v>
       </c>
       <c r="B66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="C66" s="0" t="s">
-        <v>182</v>
-      </c>
       <c r="D66" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>106</v>
@@ -2094,16 +2094,16 @@
         <v>2</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="D67" s="0" t="s">
-        <v>185</v>
+        <v>34</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>106</v>
@@ -2114,16 +2114,16 @@
         <v>2</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>67</v>
+        <v>184</v>
       </c>
       <c r="C68" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="E68" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>106</v>
@@ -2134,13 +2134,16 @@
         <v>2</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="D69" s="0" t="s">
+        <v>69</v>
+      </c>
       <c r="E69" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>106</v>
@@ -2148,19 +2151,16 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="D70" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="E70" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>106</v>
@@ -2168,19 +2168,19 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>189</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>106</v>
@@ -2188,19 +2188,19 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="D72" s="0" t="n">
-        <v>120</v>
+      <c r="D72" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>106</v>
@@ -2211,16 +2211,16 @@
         <v>3</v>
       </c>
       <c r="B73" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>193</v>
+      <c r="D73" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>194</v>
+        <v>15</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>106</v>
@@ -2231,16 +2231,16 @@
         <v>3</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="C74" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="F74" s="0" t="s">
         <v>106</v>
@@ -2251,16 +2251,16 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="D75" s="0" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>106</v>
@@ -2271,16 +2271,16 @@
         <v>3</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>20</v>
+        <v>197</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>198</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>106</v>
@@ -2291,16 +2291,16 @@
         <v>3</v>
       </c>
       <c r="B77" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="C77" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="D77" s="0" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>202</v>
+        <v>23</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>106</v>
@@ -2308,19 +2308,19 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>73</v>
+        <v>200</v>
       </c>
       <c r="C78" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>203</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>106</v>
@@ -2331,16 +2331,16 @@
         <v>4</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="C79" s="0" t="s">
-        <v>205</v>
-      </c>
       <c r="D79" s="0" t="s">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>202</v>
+        <v>13</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>106</v>
@@ -2348,19 +2348,19 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
       <c r="C80" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="D80" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="E80" s="0" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>106</v>
@@ -2368,10 +2368,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B81" s="0" t="n">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>208</v>
@@ -2391,13 +2391,13 @@
         <v>6</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>6.2</v>
+        <v>39</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="0" t="n">
-        <v>120</v>
+      <c r="D82" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>15</v>
@@ -2408,19 +2408,19 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>48</v>
+        <v>6</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>6.2</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D83" s="0" t="s">
-        <v>12</v>
+      <c r="D83" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>106</v>
@@ -2428,19 +2428,19 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>50</v>
+        <v>6</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D84" s="0" t="s">
-        <v>52</v>
+      <c r="D84" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>106</v>
@@ -2448,19 +2448,19 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F85" s="0" t="s">
         <v>106</v>
@@ -2468,19 +2468,19 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B86" s="0" t="n">
-        <v>180</v>
+        <v>7</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="C86" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>106</v>
@@ -2490,11 +2490,11 @@
       <c r="A87" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B87" s="0" t="n">
-        <v>56</v>
+      <c r="B87" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>34</v>
@@ -2510,17 +2510,17 @@
       <c r="A88" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B88" s="0" t="s">
-        <v>217</v>
+      <c r="B88" s="0" t="n">
+        <v>56</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>219</v>
+        <v>34</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="F88" s="0" t="s">
         <v>106</v>
@@ -2528,21 +2528,41 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B89" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B90" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C90" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D90" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E89" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F89" s="0" t="s">
+      <c r="E90" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" s="0" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaning and outputs 2.0
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="225">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">SOT95P285X100-5N</t>
   </si>
   <si>
-    <t xml:space="preserve">Battery connector 89400-0220</t>
+    <t xml:space="preserve">Battery connector t   08940-10210</t>
   </si>
   <si>
     <t xml:space="preserve">BT1</t>
@@ -127,124 +127,136 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
+    <t xml:space="preserve">R68, R71, R82, R83, R84, R85, R95, R96, R97, R133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68, 68, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2, R57, R59, R61, R63, R64, R65, R111, R112, R113, R114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC817-40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1, Q2, Q3, Q4, Q7, Q12, Q19, Q20, Q22, Q25, Q26, Q28, Q47, Q48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPN General-purpose Transistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT23_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5, C7, C8, C9, C14, C22, C25, C26, C28, C30, C55, C68, C69, C70, C71, C74, C75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R69, R72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C41, C42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120, Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C43, C72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITR9909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2, U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everlight Opto Interrupter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITR9909_LONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor connector 89400-0220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1, B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor, General Kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBLP679E-RGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2, D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP7104SRC/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19, D20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red led 2V@20ma 57mcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED_TH_3MM_20MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC74HC595ADTR2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U13, U15, U17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-Bit Serial-Input/Serial or Prallel-Output Shift Register with Latched 3-State Outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">948F-01_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17, R18, R19, R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C40, C51, C52, C73</t>
+  </si>
+  <si>
     <t xml:space="preserve">1K</t>
   </si>
   <si>
-    <t xml:space="preserve">R21, R22, R23, R24, R160, R161, R162, R163, R164, R165</t>
+    <t xml:space="preserve">R21, R22, R23, R24</t>
   </si>
   <si>
     <t xml:space="preserve">22K</t>
   </si>
   <si>
-    <t xml:space="preserve">R7, R8, R9, R10, R57, R59, R61, R63, R64, R65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120, 120, 120, 120, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5, C7, C8, C9, C14, C22, C25, C26, C28, C30, C55, C68, C69, C70, C71, C74, C75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C41, C42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3, R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120, Resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C43, C72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITR9909</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2, U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Everlight Opto Interrupter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITR9909_LONG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor connector 89400-0220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1, B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor, General Kind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBLP679E-RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2, D6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WP7104SRC/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D19, D20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red led 2V@20ma 57mcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_TH_3MM_20MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BC817-40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1, Q2, Q3, Q4, Q7, Q12, Q19, Q20, Q21, Q22, Q23, Q24, Q25, Q26, Q27, Q28, Q29, Q30, Q47, Q48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPN General-purpose Transistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT23_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC74HC595ADTR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U13, U15, U17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-Bit Serial-Input/Serial or Prallel-Output Shift Register with Latched 3-State Outputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">948F-01_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R17, R18, R19, R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C40, C51, C52, C73</t>
+    <t xml:space="preserve">R7, R8, R9, R10</t>
   </si>
   <si>
     <t xml:space="preserve">R151, R152, R153, R154</t>
@@ -283,18 +295,6 @@
     <t xml:space="preserve">INDC2520X12L</t>
   </si>
   <si>
-    <t xml:space="preserve">4.7K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2, R111, R112, R113, R114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R74, R75, R76, R77, R90, R91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R68, R69, R70, R71, R72, R73</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.7nF</t>
   </si>
   <si>
@@ -319,7 +319,10 @@
     <t xml:space="preserve">120, 120, 120, 120, 120, Resistor, 120, 120</t>
   </si>
   <si>
-    <t xml:space="preserve">R82, R83, R84, R85, R95, R96, R97, R133</t>
+    <t xml:space="preserve">R70, R73, R74, R75, R76, R77, R90, R91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68, 68, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">27-21SURC/S530-A3</t>
@@ -541,21 +544,18 @@
     <t xml:space="preserve">WR-COM_USB_Micro Type B_Horizontal_SMT</t>
   </si>
   <si>
-    <t xml:space="preserve">R25, R48, R49, R108, R166, R167, R168, R169, R170, R171, R172, R173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120, 120, 120, Resistor, 120, 120, 120, 120, 120, 120, 120, 120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11, R42, R43, R67, R92, R93, R94, R130, R142, R144, R145, R146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120, 120, 120, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
+    <t xml:space="preserve">R56, R58, R60, R62, R78, R79, R80, R81, R100, R149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, 68, 68</t>
   </si>
   <si>
     <t xml:space="preserve">R135, R150</t>
   </si>
   <si>
+    <t xml:space="preserve">R99, R148</t>
+  </si>
+  <si>
     <t xml:space="preserve">R107, R137</t>
   </si>
   <si>
@@ -592,7 +592,7 @@
     <t xml:space="preserve">C1, C3, C6, C10, C11, C12, C13, C23, C24, C27, C29, C33, C35, C36, C37, C38, C39, C62, C65, C66, C67</t>
   </si>
   <si>
-    <t xml:space="preserve">Q5, Q6, Q8, Q9, Q10, Q11, Q13, Q14, Q15, Q16, Q17, Q18, Q31, Q32, Q33, Q34, Q35, Q36, Q37, Q38, Q39, Q40, Q41, Q42, Q43, Q44, Q45, Q46</t>
+    <t xml:space="preserve">Q5, Q6, Q8, Q9, Q10, Q11, Q13, Q14, Q15, Q16, Q17, Q18, Q31, Q32, Q34, Q37, Q38, Q39, Q40, Q42, Q45, Q46</t>
   </si>
   <si>
     <t xml:space="preserve">R26, R46, R47</t>
@@ -619,9 +619,6 @@
     <t xml:space="preserve">C58, C59, C60</t>
   </si>
   <si>
-    <t xml:space="preserve">U18, U22, U24</t>
-  </si>
-  <si>
     <t xml:space="preserve">APTD1608CGCK</t>
   </si>
   <si>
@@ -634,9 +631,6 @@
     <t xml:space="preserve">DIOC1608X08N</t>
   </si>
   <si>
-    <t xml:space="preserve">C2, C4, C31, C46</t>
-  </si>
-  <si>
     <t xml:space="preserve">19-21SURC/S530-A3/TR8</t>
   </si>
   <si>
@@ -646,21 +640,33 @@
     <t xml:space="preserve">SMD Red 0603 2V@20ma 56 mcd</t>
   </si>
   <si>
+    <t xml:space="preserve">U18, U22, U24, U27</t>
+  </si>
+  <si>
     <t xml:space="preserve">R138, R139, R141, R143, R159</t>
   </si>
   <si>
-    <t xml:space="preserve">R66, R86, R87, R88, R89, R134</t>
+    <t xml:space="preserve">C2, C4, C31, C46, C76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25, R48, R49, R108, R166, R167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120, 120, 120, Resistor, 120, 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11, R42, R43, R67, R130, R142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120, 120, 120, Resistor, Resistor, Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R92, R93, R94, R144, R145, R146</t>
   </si>
   <si>
     <t xml:space="preserve">R36, R37, R39, R40, R54, R55</t>
   </si>
   <si>
-    <t xml:space="preserve">R98, R99, R100, R147, R148, R149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C32, C44, C45, C47, C48, C49, C50</t>
-  </si>
-  <si>
     <t xml:space="preserve">U6, U7, U8, U9, U10, U11, U12</t>
   </si>
   <si>
@@ -670,7 +676,13 @@
     <t xml:space="preserve">R101, R102, R109, R110, R117, R118, R128, R129</t>
   </si>
   <si>
-    <t xml:space="preserve">R56, R58, R60, R62, R78, R79, R80, R81</t>
+    <t xml:space="preserve">R66, R86, R87, R88, R89, R98, R134, R147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor, Resistor, Resistor, Resistor, Resistor, 68, Resistor, 68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C32, C44, C45, C47, C48, C49, C50, C77</t>
   </si>
   <si>
     <t xml:space="preserve">APTD1608SYCK</t>
@@ -778,7 +790,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -788,7 +800,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="120.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.41"/>
@@ -979,14 +991,14 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>120</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>15</v>
@@ -997,7 +1009,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>37</v>
@@ -1006,7 +1018,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>15</v>
@@ -1017,19 +1029,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>9</v>
@@ -1037,13 +1049,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>13</v>
@@ -1056,14 +1071,14 @@
       <c r="A15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>44</v>
+      <c r="B15" s="0" t="n">
+        <v>150</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>34</v>
+      <c r="D15" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>15</v>
@@ -1076,17 +1091,14 @@
       <c r="A16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>33</v>
+      <c r="B16" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>9</v>
@@ -1103,10 +1115,10 @@
         <v>49</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>9</v>
@@ -1116,17 +1128,17 @@
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="E18" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>9</v>
@@ -1137,16 +1149,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>9</v>
@@ -1157,10 +1169,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>57</v>
@@ -1174,16 +1189,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="E21" s="0" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>9</v>
@@ -1191,19 +1206,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>9</v>
@@ -1211,19 +1223,19 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>9</v>
@@ -1231,19 +1243,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>120</v>
+        <v>68</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>9</v>
@@ -1254,16 +1266,16 @@
         <v>4</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>12</v>
+        <v>72</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>9</v>
@@ -1273,17 +1285,17 @@
       <c r="A26" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B26" s="0" t="n">
-        <v>820</v>
+      <c r="B26" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>9</v>
@@ -1294,16 +1306,16 @@
         <v>4</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>78</v>
+      <c r="D27" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>9</v>
@@ -1314,16 +1326,16 @@
         <v>4</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>9</v>
@@ -1333,17 +1345,17 @@
       <c r="A29" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>83</v>
+      <c r="B29" s="0" t="n">
+        <v>820</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>9</v>
@@ -1351,19 +1363,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>9</v>
@@ -1371,19 +1383,19 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>9</v>
@@ -1391,19 +1403,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>68</v>
+        <v>4</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>68</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>9</v>
@@ -1474,13 +1486,13 @@
         <v>8</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>99</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>15</v>
@@ -1494,16 +1506,16 @@
         <v>9</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>9</v>
@@ -1514,10 +1526,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>12</v>
@@ -1526,7 +1538,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1549,7 @@
         <v>100</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>
@@ -1546,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>12</v>
@@ -1566,7 +1578,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>34</v>
@@ -1586,7 +1598,7 @@
         <v>15</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>34</v>
@@ -1606,7 +1618,7 @@
         <v>15</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,10 +1626,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>12</v>
@@ -1626,7 +1638,7 @@
         <v>13</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,10 +1646,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>34</v>
@@ -1646,7 +1658,7 @@
         <v>15</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,10 +1666,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>34</v>
@@ -1666,7 +1678,7 @@
         <v>15</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1677,7 +1689,7 @@
         <v>820</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>34</v>
@@ -1686,7 +1698,7 @@
         <v>15</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,19 +1706,19 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,19 +1726,19 @@
         <v>1</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,19 +1746,19 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,19 +1766,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,7 +1789,7 @@
         <v>28</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>30</v>
@@ -1786,7 +1798,7 @@
         <v>31</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,19 +1806,19 @@
         <v>1</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,19 +1826,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,19 +1846,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,19 +1866,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,19 +1886,19 @@
         <v>1</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,19 +1906,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,19 +1926,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,19 +1946,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,59 +1966,59 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>629105150521</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>56</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>176</v>
+        <v>34</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,19 +2026,19 @@
         <v>2</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>34</v>
+      <c r="D63" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,7 +2058,7 @@
         <v>15</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,7 +2078,7 @@
         <v>13</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,7 +2098,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,10 +2135,10 @@
         <v>186</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,7 +2158,7 @@
         <v>70</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,16 +2166,16 @@
         <v>2</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>188</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2183,7 @@
         <v>21</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>189</v>
@@ -2183,27 +2195,27 @@
         <v>13</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>190</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2235,7 @@
         <v>15</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2255,7 @@
         <v>195</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,19 +2263,19 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>196</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,7 +2295,7 @@
         <v>13</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,39 +2303,39 @@
         <v>3</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D78" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="E78" s="0" t="s">
-        <v>203</v>
-      </c>
       <c r="F78" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,39 +2343,39 @@
         <v>4</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>207</v>
+        <v>34</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>203</v>
+        <v>15</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,99 +2383,99 @@
         <v>5</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>208</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B82" s="0" t="n">
-        <v>39</v>
+      <c r="B82" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>209</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>34</v>
+        <v>210</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B83" s="0" t="n">
-        <v>6.2</v>
+      <c r="B83" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>120</v>
+        <v>211</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>212</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B84" s="0" t="n">
-        <v>68</v>
+      <c r="B84" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>68</v>
+        <v>213</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>48</v>
+        <v>6</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>6.2</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>12</v>
+        <v>214</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,19 +2483,19 @@
         <v>7</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,7 +2506,7 @@
         <v>93</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>34</v>
@@ -2503,7 +2515,7 @@
         <v>15</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,19 +2523,19 @@
         <v>8</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>34</v>
+        <v>219</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,39 +2543,59 @@
         <v>8</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>217</v>
+        <v>52</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C90" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D90" s="0" t="s">
+      <c r="C91" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D91" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E90" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F90" s="0" t="s">
-        <v>106</v>
+      <c r="E91" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change resistor led value change shift register outputs 2.01
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="225">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -127,12 +127,6 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R68, R71, R82, R83, R84, R85, R95, R96, R97, R133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68, 68, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.7K</t>
   </si>
   <si>
@@ -157,21 +151,21 @@
     <t xml:space="preserve">C5, C7, C8, C9, C14, C22, C25, C26, C28, C30, C55, C68, C69, C70, C71, C74, C75</t>
   </si>
   <si>
+    <t xml:space="preserve">18pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C41, C42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R6</t>
+  </si>
+  <si>
     <t xml:space="preserve">R69, R72</t>
   </si>
   <si>
-    <t xml:space="preserve">18pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C41, C42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R6</t>
-  </si>
-  <si>
     <t xml:space="preserve">R3, R5</t>
   </si>
   <si>
@@ -184,6 +178,9 @@
     <t xml:space="preserve">C43, C72</t>
   </si>
   <si>
+    <t xml:space="preserve">R70, R73</t>
+  </si>
+  <si>
     <t xml:space="preserve">ITR9909</t>
   </si>
   <si>
@@ -223,7 +220,7 @@
     <t xml:space="preserve">LED_TH_3MM_20MM</t>
   </si>
   <si>
-    <t xml:space="preserve">MC74HC595ADTR2G</t>
+    <t xml:space="preserve">SN74HC595PWR</t>
   </si>
   <si>
     <t xml:space="preserve">U13, U15, U17</t>
@@ -319,10 +316,13 @@
     <t xml:space="preserve">120, 120, 120, 120, 120, Resistor, 120, 120</t>
   </si>
   <si>
-    <t xml:space="preserve">R70, R73, R74, R75, R76, R77, R90, R91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68, 68, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
+    <t xml:space="preserve">R82, R83, R84, R85, R95, R96, R97, R133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R68, R71, R74, R75, R76, R77, R90, R91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56, 56, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">27-21SURC/S530-A3</t>
@@ -544,36 +544,39 @@
     <t xml:space="preserve">WR-COM_USB_Micro Type B_Horizontal_SMT</t>
   </si>
   <si>
-    <t xml:space="preserve">R56, R58, R60, R62, R78, R79, R80, R81, R100, R149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, 68, 68</t>
+    <t xml:space="preserve">R56, R58, R60, R62, R78, R79, R80, R81, R98, R147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, Resistor, 56, 56</t>
   </si>
   <si>
     <t xml:space="preserve">R135, R150</t>
   </si>
   <si>
+    <t xml:space="preserve">R107, R137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C53, C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C56, C61</t>
+  </si>
+  <si>
     <t xml:space="preserve">R99, R148</t>
   </si>
   <si>
-    <t xml:space="preserve">R107, R137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C53, C54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C56, C61</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.6K</t>
   </si>
   <si>
     <t xml:space="preserve">R115, R116</t>
   </si>
   <si>
+    <t xml:space="preserve">R100, R149</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAT54S</t>
   </si>
   <si>
@@ -583,12 +586,12 @@
     <t xml:space="preserve">Schottky Barrier Double Diode</t>
   </si>
   <si>
+    <t xml:space="preserve">D27, D38</t>
+  </si>
+  <si>
     <t xml:space="preserve">U14, U16</t>
   </si>
   <si>
-    <t xml:space="preserve">D27, D38</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1, C3, C6, C10, C11, C12, C13, C23, C24, C27, C29, C33, C35, C36, C37, C38, C39, C62, C65, C66, C67</t>
   </si>
   <si>
@@ -661,6 +664,9 @@
     <t xml:space="preserve">120, 120, 120, Resistor, Resistor, Resistor</t>
   </si>
   <si>
+    <t xml:space="preserve">R66, R86, R87, R88, R89, R134</t>
+  </si>
+  <si>
     <t xml:space="preserve">R92, R93, R94, R144, R145, R146</t>
   </si>
   <si>
@@ -674,12 +680,6 @@
   </si>
   <si>
     <t xml:space="preserve">R101, R102, R109, R110, R117, R118, R128, R129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R66, R86, R87, R88, R89, R98, R134, R147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, Resistor, Resistor, Resistor, Resistor, 68, Resistor, 68</t>
   </si>
   <si>
     <t xml:space="preserve">C32, C44, C45, C47, C48, C49, C50, C77</t>
@@ -790,7 +790,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -798,13 +798,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,16 +989,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>15</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>37</v>
@@ -1018,10 +1018,10 @@
         <v>38</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>9</v>
@@ -1029,19 +1029,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>9</v>
@@ -1049,16 +1049,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>13</v>
@@ -1071,14 +1068,14 @@
       <c r="A15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>150</v>
+      <c r="B15" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>68</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>15</v>
@@ -1091,14 +1088,17 @@
       <c r="A16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>46</v>
+      <c r="B16" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>200</v>
+      </c>
       <c r="E16" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>9</v>
@@ -1108,14 +1108,14 @@
       <c r="A17" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>15</v>
@@ -1128,17 +1128,17 @@
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>33</v>
+      <c r="B18" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>9</v>
@@ -1148,17 +1148,17 @@
       <c r="A19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>12</v>
+      <c r="D19" s="0" t="n">
+        <v>82</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>9</v>
@@ -1169,16 +1169,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>9</v>
@@ -1189,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>27</v>
@@ -1209,13 +1209,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E22" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>9</v>
@@ -1226,16 +1226,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>9</v>
@@ -1246,16 +1246,16 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>9</v>
@@ -1266,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>120</v>
@@ -1286,10 +1286,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>12</v>
@@ -1306,10 +1306,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>120</v>
@@ -1326,10 +1326,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>120</v>
@@ -1349,7 +1349,7 @@
         <v>820</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>34</v>
@@ -1366,16 +1366,16 @@
         <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>9</v>
@@ -1386,16 +1386,16 @@
         <v>4</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="E31" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>9</v>
@@ -1406,16 +1406,16 @@
         <v>4</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>9</v>
@@ -1426,10 +1426,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>12</v>
@@ -1446,13 +1446,13 @@
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>15</v>
@@ -1466,13 +1466,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>15</v>
@@ -1486,13 +1486,13 @@
         <v>8</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>15</v>
@@ -1503,19 +1503,19 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>101</v>
+        <v>8</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>56</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>9</v>
@@ -1523,39 +1523,39 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>100</v>
+      <c r="B39" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>107</v>
@@ -1565,17 +1565,17 @@
       <c r="A40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>109</v>
+      <c r="B40" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>107</v>
@@ -1586,16 +1586,16 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>107</v>
@@ -1606,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>34</v>
@@ -1626,16 +1626,16 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>107</v>
@@ -1646,16 +1646,16 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>107</v>
@@ -1666,10 +1666,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>34</v>
@@ -1685,11 +1685,11 @@
       <c r="A46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>820</v>
+      <c r="B46" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>34</v>
@@ -1705,17 +1705,17 @@
       <c r="A47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>122</v>
+      <c r="B47" s="0" t="n">
+        <v>820</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>107</v>
@@ -1726,16 +1726,16 @@
         <v>1</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>107</v>
@@ -1746,16 +1746,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>107</v>
@@ -1766,16 +1766,16 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>107</v>
@@ -1786,16 +1786,16 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>107</v>
@@ -1806,16 +1806,16 @@
         <v>1</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>107</v>
@@ -1826,16 +1826,16 @@
         <v>1</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>107</v>
@@ -1846,16 +1846,16 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>107</v>
@@ -1866,16 +1866,16 @@
         <v>1</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>107</v>
@@ -1886,16 +1886,16 @@
         <v>1</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>107</v>
@@ -1906,16 +1906,16 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>107</v>
@@ -1926,16 +1926,16 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>107</v>
@@ -1946,16 +1946,16 @@
         <v>1</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>107</v>
@@ -1966,16 +1966,16 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E60" s="0" t="n">
-        <v>629105150521</v>
+        <v>169</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>170</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>107</v>
@@ -1983,19 +1983,19 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>171</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>15</v>
+        <v>173</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>629105150521</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>107</v>
@@ -2003,16 +2003,16 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>15</v>
@@ -2026,13 +2026,13 @@
         <v>2</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="D63" s="0" t="n">
-        <v>68</v>
+        <v>176</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>15</v>
@@ -2049,7 +2049,7 @@
         <v>180</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>34</v>
@@ -2066,10 +2066,10 @@
         <v>2</v>
       </c>
       <c r="B65" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>180</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>12</v>
@@ -2089,7 +2089,7 @@
         <v>10</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>12</v>
@@ -2105,14 +2105,14 @@
       <c r="A67" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>182</v>
+      <c r="B67" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>34</v>
+        <v>181</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>15</v>
@@ -2126,16 +2126,16 @@
         <v>2</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>107</v>
@@ -2145,17 +2145,17 @@
       <c r="A69" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>67</v>
+      <c r="B69" s="0" t="n">
+        <v>82</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>69</v>
+        <v>184</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>82</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>107</v>
@@ -2166,13 +2166,16 @@
         <v>2</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>107</v>
@@ -2180,19 +2183,16 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>12</v>
+        <v>188</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>107</v>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>107</v>
@@ -2220,19 +2220,19 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>120</v>
+        <v>190</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>107</v>
@@ -2240,19 +2240,19 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>192</v>
+        <v>37</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>194</v>
+        <v>39</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>195</v>
+        <v>40</v>
       </c>
       <c r="F74" s="0" t="s">
         <v>107</v>
@@ -2263,16 +2263,16 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>103</v>
+        <v>192</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>107</v>
@@ -2283,16 +2283,16 @@
         <v>3</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>107</v>
@@ -2303,16 +2303,16 @@
         <v>3</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>199</v>
+        <v>101</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>201</v>
+        <v>103</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>107</v>
@@ -2320,19 +2320,19 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>205</v>
+        <v>12</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>202</v>
+        <v>13</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>107</v>
@@ -2340,19 +2340,19 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>23</v>
+        <v>203</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>107</v>
@@ -2360,19 +2360,19 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>32</v>
+        <v>204</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>107</v>
@@ -2380,19 +2380,19 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>107</v>
@@ -2400,16 +2400,16 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>210</v>
+        <v>34</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>15</v>
@@ -2420,19 +2420,19 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>212</v>
+        <v>12</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>107</v>
@@ -2443,13 +2443,13 @@
         <v>6</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>15</v>
@@ -2462,14 +2462,14 @@
       <c r="A85" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B85" s="0" t="n">
-        <v>6.2</v>
+      <c r="B85" s="0" t="s">
+        <v>76</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>120</v>
+        <v>212</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>213</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>15</v>
@@ -2480,19 +2480,19 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>54</v>
+        <v>6</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>39</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>216</v>
+        <v>15</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>107</v>
@@ -2500,13 +2500,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>34</v>
@@ -2520,16 +2520,16 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>39</v>
+        <v>6.2</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>219</v>
+        <v>216</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>15</v>
@@ -2540,19 +2540,19 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>107</v>
@@ -2563,16 +2563,16 @@
         <v>8</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>221</v>
+        <v>92</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>223</v>
+        <v>34</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>107</v>
@@ -2580,21 +2580,61 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C91" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D93" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E91" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F91" s="0" t="s">
+      <c r="E93" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93" s="0" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generate 2.1 output files
</commit_message>
<xml_diff>
--- a/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials by layers-thymio2-main(Production Thymio2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="226">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -238,58 +238,58 @@
     <t xml:space="preserve">R17, R18, R19, R20</t>
   </si>
   <si>
+    <t xml:space="preserve">1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21, R22, R23, R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7, R8, R9, R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2508056017Y2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1, L2, L3, L4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD EMI Suppression Ferrite Bead WE-CBF, Z = 600 Ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDC2012X11L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R151, R152, R153, R154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMG1012T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T5, T6, T7, T8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transistor MOSFET 1 x N, Pining : 1=G, 2=S, 3=D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT50P160X80-3N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMP21DOUT-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T1, T2, T3, T4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transistor MOSFET 1 x P Pining : 1=G, 2=S, 3=D</t>
+  </si>
+  <si>
     <t xml:space="preserve">10uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C40, C51, C52, C73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21, R22, R23, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7, R8, R9, R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R151, R152, R153, R154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMG1012T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T5, T6, T7, T8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transistor MOSFET 1 x N, Pining : 1=G, 2=S, 3=D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT50P160X80-3N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMP21DOUT-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1, T2, T3, T4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transistor MOSFET 1 x P Pining : 1=G, 2=S, 3=D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLP2520S3R3S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L1, L2, L3, L4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductors for Power Circuits  Multilayer/STD  Magnetic Shielded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDC2520X12L</t>
+    <t xml:space="preserve">C40, C51, C52, C73, C78</t>
   </si>
   <si>
     <t xml:space="preserve">4.7nF</t>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">C34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5</t>
   </si>
   <si>
     <t xml:space="preserve">270K</t>
@@ -790,7 +793,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -798,13 +801,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,11 +1294,11 @@
       <c r="C26" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>12</v>
+      <c r="D26" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>9</v>
@@ -1331,11 +1334,11 @@
       <c r="C28" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>120</v>
+      <c r="D28" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>9</v>
@@ -1349,7 +1352,7 @@
         <v>820</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>34</v>
@@ -1366,16 +1369,16 @@
         <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>9</v>
@@ -1386,16 +1389,16 @@
         <v>4</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>9</v>
@@ -1403,19 +1406,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>9</v>
@@ -1606,16 +1609,16 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="D42" s="0" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>107</v>
@@ -1626,10 +1629,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>34</v>
@@ -1646,16 +1649,16 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="D44" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>107</v>
@@ -1666,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="D45" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>107</v>
@@ -1686,10 +1689,10 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>34</v>
@@ -1705,8 +1708,8 @@
       <c r="A47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>820</v>
+      <c r="B47" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>121</v>
@@ -1725,17 +1728,17 @@
       <c r="A48" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="0" t="n">
+        <v>820</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="D48" s="0" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>107</v>
@@ -1746,16 +1749,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>107</v>
@@ -1766,16 +1769,16 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>107</v>
@@ -1786,16 +1789,16 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>137</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>107</v>
@@ -1806,16 +1809,16 @@
         <v>1</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>107</v>
@@ -1826,16 +1829,16 @@
         <v>1</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="D53" s="0" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>107</v>
@@ -1846,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>146</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>107</v>
@@ -1866,16 +1869,16 @@
         <v>1</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>150</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>107</v>
@@ -1886,16 +1889,16 @@
         <v>1</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>154</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>107</v>
@@ -1906,16 +1909,16 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>158</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>107</v>
@@ -1926,16 +1929,16 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>107</v>
@@ -1946,16 +1949,16 @@
         <v>1</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>166</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>107</v>
@@ -1966,16 +1969,16 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>107</v>
@@ -1986,16 +1989,16 @@
         <v>1</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61" s="0" t="n">
-        <v>629105150521</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>107</v>
@@ -2003,19 +2006,19 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>172</v>
       </c>
       <c r="C62" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>15</v>
+      <c r="E62" s="0" t="n">
+        <v>629105150521</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>107</v>
@@ -2023,16 +2026,16 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C63" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D63" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>15</v>
@@ -2046,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>177</v>
@@ -2065,17 +2068,17 @@
       <c r="A65" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="0" t="s">
-        <v>179</v>
-      </c>
       <c r="D65" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>107</v>
@@ -2086,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>180</v>
@@ -2105,17 +2108,17 @@
       <c r="A67" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B67" s="0" t="n">
-        <v>200</v>
+      <c r="B67" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="D67" s="0" t="n">
-        <v>200</v>
+      <c r="D67" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>107</v>
@@ -2125,14 +2128,14 @@
       <c r="A68" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C68" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>34</v>
+      <c r="D68" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>15</v>
@@ -2145,14 +2148,14 @@
       <c r="A69" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B69" s="0" t="n">
-        <v>82</v>
+      <c r="B69" s="0" t="s">
+        <v>183</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="D69" s="0" t="n">
-        <v>82</v>
+      <c r="D69" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>15</v>
@@ -2165,17 +2168,17 @@
       <c r="A70" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C70" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>187</v>
+      <c r="D70" s="0" t="n">
+        <v>82</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>107</v>
@@ -2186,13 +2189,16 @@
         <v>2</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>60</v>
+        <v>186</v>
       </c>
       <c r="C71" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" s="0" t="s">
         <v>188</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>107</v>
@@ -2203,16 +2209,13 @@
         <v>2</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D72" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="E72" s="0" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>107</v>
@@ -2220,19 +2223,19 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>190</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>107</v>
@@ -2240,19 +2243,19 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>191</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="F74" s="0" t="s">
         <v>107</v>
@@ -2260,19 +2263,19 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="D75" s="0" t="n">
-        <v>120</v>
+      <c r="D75" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>107</v>
@@ -2283,16 +2286,16 @@
         <v>3</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>195</v>
+      <c r="D76" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>107</v>
@@ -2303,16 +2306,16 @@
         <v>3</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="C77" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E77" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>107</v>
@@ -2323,16 +2326,16 @@
         <v>3</v>
       </c>
       <c r="B78" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>199</v>
-      </c>
       <c r="D78" s="0" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>107</v>
@@ -2343,16 +2346,16 @@
         <v>3</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="0" t="s">
-        <v>201</v>
-      </c>
       <c r="D79" s="0" t="s">
-        <v>202</v>
+        <v>12</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>107</v>
@@ -2360,19 +2363,19 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E80" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>203</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>107</v>
@@ -2383,16 +2386,16 @@
         <v>4</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>20</v>
+        <v>205</v>
       </c>
       <c r="C81" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="D81" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E81" s="0" t="s">
-        <v>23</v>
+        <v>204</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>107</v>
@@ -2400,19 +2403,19 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>208</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>107</v>
@@ -2423,16 +2426,16 @@
         <v>5</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>209</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>107</v>
@@ -2440,19 +2443,19 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>210</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>211</v>
+        <v>12</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>107</v>
@@ -2463,13 +2466,13 @@
         <v>6</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C85" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>212</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>213</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>15</v>
@@ -2482,14 +2485,14 @@
       <c r="A86" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B86" s="0" t="n">
-        <v>39</v>
+      <c r="B86" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="C86" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>15</v>
@@ -2502,8 +2505,8 @@
       <c r="A87" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>35</v>
+      <c r="B87" s="0" t="n">
+        <v>39</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>215</v>
@@ -2522,14 +2525,14 @@
       <c r="A88" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B88" s="0" t="n">
-        <v>6.2</v>
+      <c r="B88" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D88" s="0" t="n">
-        <v>120</v>
+      <c r="D88" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>15</v>
@@ -2540,19 +2543,19 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>6.2</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="D89" s="0" t="s">
-        <v>55</v>
+      <c r="D89" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>218</v>
+        <v>15</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>107</v>
@@ -2560,19 +2563,19 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="C90" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E90" s="0" t="s">
         <v>219</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>107</v>
@@ -2583,16 +2586,16 @@
         <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>220</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>107</v>
@@ -2603,16 +2606,16 @@
         <v>8</v>
       </c>
       <c r="B92" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="C92" s="0" t="s">
-        <v>222</v>
-      </c>
       <c r="D92" s="0" t="s">
-        <v>223</v>
+        <v>12</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>107</v>
@@ -2620,21 +2623,41 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C93" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="D93" s="0" t="s">
+      <c r="C94" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E93" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F93" s="0" t="s">
+      <c r="E94" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="0" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>